<commit_message>
Distrubicuion normal de las posiciones networkX
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -465,13 +465,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1000000</v>
+        <v>10000</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>1e-06</v>
+        <v>0.0001</v>
       </c>
       <c r="E2" t="inlineStr"/>
     </row>
@@ -480,13 +480,13 @@
         <v>0.01</v>
       </c>
       <c r="B3" t="n">
-        <v>999795</v>
+        <v>9989</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>2e-06</v>
+        <v>0.0003</v>
       </c>
       <c r="E3" t="inlineStr"/>
     </row>
@@ -495,13 +495,13 @@
         <v>0.02</v>
       </c>
       <c r="B4" t="n">
-        <v>999212</v>
+        <v>9963</v>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D4" t="n">
-        <v>3e-06</v>
+        <v>0.0009</v>
       </c>
       <c r="E4" t="inlineStr"/>
     </row>
@@ -510,13 +510,13 @@
         <v>0.03</v>
       </c>
       <c r="B5" t="n">
-        <v>998242</v>
+        <v>9911</v>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D5" t="n">
-        <v>4e-06</v>
+        <v>0.0013</v>
       </c>
       <c r="E5" t="inlineStr"/>
     </row>
@@ -525,13 +525,13 @@
         <v>0.04</v>
       </c>
       <c r="B6" t="n">
-        <v>996862</v>
+        <v>9851</v>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D6" t="n">
-        <v>4e-06</v>
+        <v>0.0013</v>
       </c>
       <c r="E6" t="inlineStr"/>
     </row>
@@ -540,13 +540,13 @@
         <v>0.05</v>
       </c>
       <c r="B7" t="n">
-        <v>995161</v>
+        <v>9774</v>
       </c>
       <c r="C7" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D7" t="n">
-        <v>5e-06</v>
+        <v>0.0013</v>
       </c>
       <c r="E7" t="inlineStr"/>
     </row>
@@ -555,13 +555,13 @@
         <v>0.06</v>
       </c>
       <c r="B8" t="n">
-        <v>992945</v>
+        <v>9686</v>
       </c>
       <c r="C8" t="n">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D8" t="n">
-        <v>6e-06</v>
+        <v>0.0017</v>
       </c>
       <c r="E8" t="inlineStr"/>
     </row>
@@ -570,13 +570,13 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="B9" t="n">
-        <v>990336</v>
+        <v>9585</v>
       </c>
       <c r="C9" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D9" t="n">
-        <v>6e-06</v>
+        <v>0.0025</v>
       </c>
       <c r="E9" t="inlineStr"/>
     </row>
@@ -585,13 +585,13 @@
         <v>0.08</v>
       </c>
       <c r="B10" t="n">
-        <v>987350</v>
+        <v>9498</v>
       </c>
       <c r="C10" t="n">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D10" t="n">
-        <v>1e-05</v>
+        <v>0.0028</v>
       </c>
       <c r="E10" t="inlineStr"/>
     </row>
@@ -600,13 +600,13 @@
         <v>0.09</v>
       </c>
       <c r="B11" t="n">
-        <v>984040</v>
+        <v>9412</v>
       </c>
       <c r="C11" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D11" t="n">
-        <v>1e-05</v>
+        <v>0.005</v>
       </c>
       <c r="E11" t="inlineStr"/>
     </row>
@@ -615,13 +615,13 @@
         <v>0.1</v>
       </c>
       <c r="B12" t="n">
-        <v>980395</v>
+        <v>9324</v>
       </c>
       <c r="C12" t="n">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="D12" t="n">
-        <v>1e-05</v>
+        <v>0.0065</v>
       </c>
       <c r="E12" t="inlineStr"/>
     </row>
@@ -630,13 +630,13 @@
         <v>0.11</v>
       </c>
       <c r="B13" t="n">
-        <v>976193</v>
+        <v>9236</v>
       </c>
       <c r="C13" t="n">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="D13" t="n">
-        <v>1e-05</v>
+        <v>0.008200000000000001</v>
       </c>
       <c r="E13" t="inlineStr"/>
     </row>
@@ -645,13 +645,13 @@
         <v>0.12</v>
       </c>
       <c r="B14" t="n">
-        <v>971589</v>
+        <v>9145</v>
       </c>
       <c r="C14" t="n">
-        <v>10</v>
+        <v>378</v>
       </c>
       <c r="D14" t="n">
-        <v>1e-05</v>
+        <v>0.0378</v>
       </c>
       <c r="E14" t="inlineStr"/>
     </row>
@@ -660,13 +660,13 @@
         <v>0.13</v>
       </c>
       <c r="B15" t="n">
-        <v>966714</v>
+        <v>9043</v>
       </c>
       <c r="C15" t="n">
-        <v>13</v>
+        <v>438</v>
       </c>
       <c r="D15" t="n">
-        <v>1.3e-05</v>
+        <v>0.0438</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -675,13 +675,13 @@
         <v>0.14</v>
       </c>
       <c r="B16" t="n">
-        <v>961459</v>
+        <v>8930</v>
       </c>
       <c r="C16" t="n">
-        <v>18</v>
+        <v>559</v>
       </c>
       <c r="D16" t="n">
-        <v>1.8e-05</v>
+        <v>0.0559</v>
       </c>
       <c r="E16" t="inlineStr"/>
     </row>
@@ -690,13 +690,13 @@
         <v>0.15</v>
       </c>
       <c r="B17" t="n">
-        <v>955798</v>
+        <v>8827</v>
       </c>
       <c r="C17" t="n">
-        <v>18</v>
+        <v>699</v>
       </c>
       <c r="D17" t="n">
-        <v>1.8e-05</v>
+        <v>0.0699</v>
       </c>
       <c r="E17" t="inlineStr"/>
     </row>
@@ -705,13 +705,13 @@
         <v>0.16</v>
       </c>
       <c r="B18" t="n">
-        <v>949650</v>
+        <v>8734</v>
       </c>
       <c r="C18" t="n">
-        <v>18</v>
+        <v>868</v>
       </c>
       <c r="D18" t="n">
-        <v>1.8e-05</v>
+        <v>0.0868</v>
       </c>
       <c r="E18" t="inlineStr"/>
     </row>
@@ -720,13 +720,13 @@
         <v>0.17</v>
       </c>
       <c r="B19" t="n">
-        <v>943473</v>
+        <v>8599</v>
       </c>
       <c r="C19" t="n">
-        <v>18</v>
+        <v>950</v>
       </c>
       <c r="D19" t="n">
-        <v>1.8e-05</v>
+        <v>0.095</v>
       </c>
       <c r="E19" t="inlineStr"/>
     </row>
@@ -735,13 +735,13 @@
         <v>0.18</v>
       </c>
       <c r="B20" t="n">
-        <v>936790</v>
+        <v>8492</v>
       </c>
       <c r="C20" t="n">
-        <v>18</v>
+        <v>1111</v>
       </c>
       <c r="D20" t="n">
-        <v>1.8e-05</v>
+        <v>0.1111</v>
       </c>
       <c r="E20" t="inlineStr"/>
     </row>
@@ -750,13 +750,13 @@
         <v>0.19</v>
       </c>
       <c r="B21" t="n">
-        <v>929689</v>
+        <v>8377</v>
       </c>
       <c r="C21" t="n">
-        <v>19</v>
+        <v>1187</v>
       </c>
       <c r="D21" t="n">
-        <v>1.9e-05</v>
+        <v>0.1187</v>
       </c>
       <c r="E21" t="inlineStr"/>
     </row>
@@ -765,13 +765,13 @@
         <v>0.2</v>
       </c>
       <c r="B22" t="n">
-        <v>922254</v>
+        <v>8286</v>
       </c>
       <c r="C22" t="n">
-        <v>22</v>
+        <v>1288</v>
       </c>
       <c r="D22" t="n">
-        <v>2.2e-05</v>
+        <v>0.1288</v>
       </c>
       <c r="E22" t="inlineStr"/>
     </row>
@@ -780,13 +780,13 @@
         <v>0.21</v>
       </c>
       <c r="B23" t="n">
-        <v>914467</v>
+        <v>8198</v>
       </c>
       <c r="C23" t="n">
-        <v>24</v>
+        <v>1384</v>
       </c>
       <c r="D23" t="n">
-        <v>2.4e-05</v>
+        <v>0.1384</v>
       </c>
       <c r="E23" t="inlineStr"/>
     </row>
@@ -795,13 +795,13 @@
         <v>0.22</v>
       </c>
       <c r="B24" t="n">
-        <v>906210</v>
+        <v>8097</v>
       </c>
       <c r="C24" t="n">
-        <v>24</v>
+        <v>1445</v>
       </c>
       <c r="D24" t="n">
-        <v>2.4e-05</v>
+        <v>0.1445</v>
       </c>
       <c r="E24" t="inlineStr"/>
     </row>
@@ -810,13 +810,13 @@
         <v>0.23</v>
       </c>
       <c r="B25" t="n">
-        <v>897784</v>
+        <v>8001</v>
       </c>
       <c r="C25" t="n">
-        <v>24</v>
+        <v>1522</v>
       </c>
       <c r="D25" t="n">
-        <v>2.4e-05</v>
+        <v>0.1522</v>
       </c>
       <c r="E25" t="inlineStr"/>
     </row>
@@ -825,13 +825,13 @@
         <v>0.24</v>
       </c>
       <c r="B26" t="n">
-        <v>889110</v>
+        <v>7908</v>
       </c>
       <c r="C26" t="n">
-        <v>25</v>
+        <v>1651</v>
       </c>
       <c r="D26" t="n">
-        <v>2.5e-05</v>
+        <v>0.1651</v>
       </c>
       <c r="E26" t="inlineStr"/>
     </row>
@@ -840,13 +840,13 @@
         <v>0.25</v>
       </c>
       <c r="B27" t="n">
-        <v>879940</v>
+        <v>7814</v>
       </c>
       <c r="C27" t="n">
-        <v>26</v>
+        <v>1775</v>
       </c>
       <c r="D27" t="n">
-        <v>2.6e-05</v>
+        <v>0.1775</v>
       </c>
       <c r="E27" t="inlineStr"/>
     </row>
@@ -855,13 +855,13 @@
         <v>0.26</v>
       </c>
       <c r="B28" t="n">
-        <v>870408</v>
+        <v>7709</v>
       </c>
       <c r="C28" t="n">
-        <v>27</v>
+        <v>1840</v>
       </c>
       <c r="D28" t="n">
-        <v>2.7e-05</v>
+        <v>0.184</v>
       </c>
       <c r="E28" t="inlineStr"/>
     </row>
@@ -870,13 +870,13 @@
         <v>0.27</v>
       </c>
       <c r="B29" t="n">
-        <v>860288</v>
+        <v>7634</v>
       </c>
       <c r="C29" t="n">
-        <v>32</v>
+        <v>1952</v>
       </c>
       <c r="D29" t="n">
-        <v>3.2e-05</v>
+        <v>0.1952</v>
       </c>
       <c r="E29" t="inlineStr"/>
     </row>
@@ -885,13 +885,13 @@
         <v>0.28</v>
       </c>
       <c r="B30" t="n">
-        <v>849906</v>
+        <v>7548</v>
       </c>
       <c r="C30" t="n">
-        <v>32</v>
+        <v>2012</v>
       </c>
       <c r="D30" t="n">
-        <v>3.2e-05</v>
+        <v>0.2012</v>
       </c>
       <c r="E30" t="inlineStr"/>
     </row>
@@ -900,13 +900,13 @@
         <v>0.29</v>
       </c>
       <c r="B31" t="n">
-        <v>839379</v>
+        <v>7449</v>
       </c>
       <c r="C31" t="n">
-        <v>33</v>
+        <v>2105</v>
       </c>
       <c r="D31" t="n">
-        <v>3.3e-05</v>
+        <v>0.2105</v>
       </c>
       <c r="E31" t="inlineStr"/>
     </row>
@@ -915,13 +915,13 @@
         <v>0.3</v>
       </c>
       <c r="B32" t="n">
-        <v>828937</v>
+        <v>7365</v>
       </c>
       <c r="C32" t="n">
-        <v>37</v>
+        <v>2200</v>
       </c>
       <c r="D32" t="n">
-        <v>3.7e-05</v>
+        <v>0.22</v>
       </c>
       <c r="E32" t="inlineStr"/>
     </row>
@@ -930,13 +930,13 @@
         <v>0.31</v>
       </c>
       <c r="B33" t="n">
-        <v>817889</v>
+        <v>7268</v>
       </c>
       <c r="C33" t="n">
-        <v>37</v>
+        <v>2273</v>
       </c>
       <c r="D33" t="n">
-        <v>3.7e-05</v>
+        <v>0.2273</v>
       </c>
       <c r="E33" t="inlineStr"/>
     </row>
@@ -945,13 +945,13 @@
         <v>0.32</v>
       </c>
       <c r="B34" t="n">
-        <v>806642</v>
+        <v>7183</v>
       </c>
       <c r="C34" t="n">
-        <v>39</v>
+        <v>2358</v>
       </c>
       <c r="D34" t="n">
-        <v>3.9e-05</v>
+        <v>0.2358</v>
       </c>
       <c r="E34" t="inlineStr"/>
     </row>
@@ -960,13 +960,13 @@
         <v>0.33</v>
       </c>
       <c r="B35" t="n">
-        <v>795164</v>
+        <v>7087</v>
       </c>
       <c r="C35" t="n">
-        <v>53</v>
+        <v>2445</v>
       </c>
       <c r="D35" t="n">
-        <v>5.3e-05</v>
+        <v>0.2445</v>
       </c>
       <c r="E35" t="inlineStr"/>
     </row>
@@ -975,13 +975,13 @@
         <v>0.34</v>
       </c>
       <c r="B36" t="n">
-        <v>783340</v>
+        <v>6987</v>
       </c>
       <c r="C36" t="n">
-        <v>54</v>
+        <v>2550</v>
       </c>
       <c r="D36" t="n">
-        <v>5.4e-05</v>
+        <v>0.255</v>
       </c>
       <c r="E36" t="inlineStr"/>
     </row>
@@ -990,13 +990,13 @@
         <v>0.35</v>
       </c>
       <c r="B37" t="n">
-        <v>771413</v>
+        <v>6886</v>
       </c>
       <c r="C37" t="n">
-        <v>56</v>
+        <v>2673</v>
       </c>
       <c r="D37" t="n">
-        <v>5.6e-05</v>
+        <v>0.2673</v>
       </c>
       <c r="E37" t="inlineStr"/>
     </row>
@@ -1005,13 +1005,13 @@
         <v>0.36</v>
       </c>
       <c r="B38" t="n">
-        <v>758831</v>
+        <v>6787</v>
       </c>
       <c r="C38" t="n">
-        <v>61</v>
+        <v>2760</v>
       </c>
       <c r="D38" t="n">
-        <v>6.1e-05</v>
+        <v>0.276</v>
       </c>
       <c r="E38" t="inlineStr"/>
     </row>
@@ -1020,13 +1020,13 @@
         <v>0.37</v>
       </c>
       <c r="B39" t="n">
-        <v>745682</v>
+        <v>6689</v>
       </c>
       <c r="C39" t="n">
-        <v>75</v>
+        <v>2838</v>
       </c>
       <c r="D39" t="n">
-        <v>7.499999999999999e-05</v>
+        <v>0.2838</v>
       </c>
       <c r="E39" t="inlineStr"/>
     </row>
@@ -1035,13 +1035,13 @@
         <v>0.38</v>
       </c>
       <c r="B40" t="n">
-        <v>732885</v>
+        <v>6587</v>
       </c>
       <c r="C40" t="n">
-        <v>88</v>
+        <v>2921</v>
       </c>
       <c r="D40" t="n">
-        <v>8.8e-05</v>
+        <v>0.2921</v>
       </c>
       <c r="E40" t="inlineStr"/>
     </row>
@@ -1050,13 +1050,13 @@
         <v>0.39</v>
       </c>
       <c r="B41" t="n">
-        <v>719830</v>
+        <v>6491</v>
       </c>
       <c r="C41" t="n">
-        <v>89</v>
+        <v>3024</v>
       </c>
       <c r="D41" t="n">
-        <v>8.899999999999999e-05</v>
+        <v>0.3024</v>
       </c>
       <c r="E41" t="inlineStr"/>
     </row>
@@ -1065,13 +1065,13 @@
         <v>0.4</v>
       </c>
       <c r="B42" t="n">
-        <v>706496</v>
+        <v>6393</v>
       </c>
       <c r="C42" t="n">
-        <v>101</v>
+        <v>3126</v>
       </c>
       <c r="D42" t="n">
-        <v>0.000101</v>
+        <v>0.3126</v>
       </c>
       <c r="E42" t="inlineStr"/>
     </row>
@@ -1080,13 +1080,13 @@
         <v>0.41</v>
       </c>
       <c r="B43" t="n">
-        <v>693071</v>
+        <v>6285</v>
       </c>
       <c r="C43" t="n">
-        <v>131</v>
+        <v>3258</v>
       </c>
       <c r="D43" t="n">
-        <v>0.000131</v>
+        <v>0.3258</v>
       </c>
       <c r="E43" t="inlineStr"/>
     </row>
@@ -1095,13 +1095,13 @@
         <v>0.42</v>
       </c>
       <c r="B44" t="n">
-        <v>679187</v>
+        <v>6188</v>
       </c>
       <c r="C44" t="n">
-        <v>134</v>
+        <v>3394</v>
       </c>
       <c r="D44" t="n">
-        <v>0.000134</v>
+        <v>0.3394</v>
       </c>
       <c r="E44" t="inlineStr"/>
     </row>
@@ -1110,13 +1110,13 @@
         <v>0.43</v>
       </c>
       <c r="B45" t="n">
-        <v>665404</v>
+        <v>6079</v>
       </c>
       <c r="C45" t="n">
-        <v>150</v>
+        <v>3473</v>
       </c>
       <c r="D45" t="n">
-        <v>0.00015</v>
+        <v>0.3473</v>
       </c>
       <c r="E45" t="inlineStr"/>
     </row>
@@ -1125,13 +1125,13 @@
         <v>0.44</v>
       </c>
       <c r="B46" t="n">
-        <v>651231</v>
+        <v>5977</v>
       </c>
       <c r="C46" t="n">
-        <v>170</v>
+        <v>3584</v>
       </c>
       <c r="D46" t="n">
-        <v>0.00017</v>
+        <v>0.3584</v>
       </c>
       <c r="E46" t="inlineStr"/>
     </row>
@@ -1140,13 +1140,13 @@
         <v>0.45</v>
       </c>
       <c r="B47" t="n">
-        <v>637276</v>
+        <v>5875</v>
       </c>
       <c r="C47" t="n">
-        <v>340</v>
+        <v>3671</v>
       </c>
       <c r="D47" t="n">
-        <v>0.00034</v>
+        <v>0.3671</v>
       </c>
       <c r="E47" t="inlineStr"/>
     </row>
@@ -1155,13 +1155,13 @@
         <v>0.46</v>
       </c>
       <c r="B48" t="n">
-        <v>623291</v>
+        <v>5769</v>
       </c>
       <c r="C48" t="n">
-        <v>350</v>
+        <v>3796</v>
       </c>
       <c r="D48" t="n">
-        <v>0.00035</v>
+        <v>0.3796</v>
       </c>
       <c r="E48" t="inlineStr"/>
     </row>
@@ -1170,13 +1170,13 @@
         <v>0.47</v>
       </c>
       <c r="B49" t="n">
-        <v>609018</v>
+        <v>5673</v>
       </c>
       <c r="C49" t="n">
-        <v>402</v>
+        <v>3915</v>
       </c>
       <c r="D49" t="n">
-        <v>0.000402</v>
+        <v>0.3915</v>
       </c>
       <c r="E49" t="inlineStr"/>
     </row>
@@ -1185,13 +1185,13 @@
         <v>0.48</v>
       </c>
       <c r="B50" t="n">
-        <v>594551</v>
+        <v>5570</v>
       </c>
       <c r="C50" t="n">
-        <v>473</v>
+        <v>4005</v>
       </c>
       <c r="D50" t="n">
-        <v>0.000473</v>
+        <v>0.4005</v>
       </c>
       <c r="E50" t="inlineStr"/>
     </row>
@@ -1200,13 +1200,13 @@
         <v>0.49</v>
       </c>
       <c r="B51" t="n">
-        <v>580027</v>
+        <v>5473</v>
       </c>
       <c r="C51" t="n">
-        <v>517</v>
+        <v>4112</v>
       </c>
       <c r="D51" t="n">
-        <v>0.000517</v>
+        <v>0.4112</v>
       </c>
       <c r="E51" t="inlineStr"/>
     </row>
@@ -1215,13 +1215,13 @@
         <v>0.5</v>
       </c>
       <c r="B52" t="n">
-        <v>565330</v>
+        <v>5360</v>
       </c>
       <c r="C52" t="n">
-        <v>557</v>
+        <v>4213</v>
       </c>
       <c r="D52" t="n">
-        <v>0.000557</v>
+        <v>0.4213</v>
       </c>
       <c r="E52" t="inlineStr"/>
     </row>
@@ -1230,13 +1230,13 @@
         <v>0.51</v>
       </c>
       <c r="B53" t="n">
-        <v>550722</v>
+        <v>5270</v>
       </c>
       <c r="C53" t="n">
-        <v>615</v>
+        <v>4329</v>
       </c>
       <c r="D53" t="n">
-        <v>0.000615</v>
+        <v>0.4329</v>
       </c>
       <c r="E53" t="inlineStr"/>
     </row>
@@ -1245,13 +1245,13 @@
         <v>0.52</v>
       </c>
       <c r="B54" t="n">
-        <v>536342</v>
+        <v>5163</v>
       </c>
       <c r="C54" t="n">
-        <v>760</v>
+        <v>4465</v>
       </c>
       <c r="D54" t="n">
-        <v>0.00076</v>
+        <v>0.4465</v>
       </c>
       <c r="E54" t="inlineStr"/>
     </row>
@@ -1260,13 +1260,13 @@
         <v>0.53</v>
       </c>
       <c r="B55" t="n">
-        <v>521925</v>
+        <v>5078</v>
       </c>
       <c r="C55" t="n">
-        <v>1076</v>
+        <v>4570</v>
       </c>
       <c r="D55" t="n">
-        <v>0.001076</v>
+        <v>0.457</v>
       </c>
       <c r="E55" t="inlineStr"/>
     </row>
@@ -1275,13 +1275,13 @@
         <v>0.54</v>
       </c>
       <c r="B56" t="n">
-        <v>507913</v>
+        <v>4979</v>
       </c>
       <c r="C56" t="n">
-        <v>1359</v>
+        <v>4642</v>
       </c>
       <c r="D56" t="n">
-        <v>0.001359</v>
+        <v>0.4642</v>
       </c>
       <c r="E56" t="inlineStr"/>
     </row>
@@ -1290,13 +1290,13 @@
         <v>0.55</v>
       </c>
       <c r="B57" t="n">
-        <v>493502</v>
+        <v>4888</v>
       </c>
       <c r="C57" t="n">
-        <v>1921</v>
+        <v>4744</v>
       </c>
       <c r="D57" t="n">
-        <v>0.001921</v>
+        <v>0.4744</v>
       </c>
       <c r="E57" t="inlineStr"/>
     </row>
@@ -1305,13 +1305,13 @@
         <v>0.5600000000000001</v>
       </c>
       <c r="B58" t="n">
-        <v>479279</v>
+        <v>4777</v>
       </c>
       <c r="C58" t="n">
-        <v>5169</v>
+        <v>4841</v>
       </c>
       <c r="D58" t="n">
-        <v>0.005169</v>
+        <v>0.4841</v>
       </c>
       <c r="E58" t="inlineStr"/>
     </row>
@@ -1320,13 +1320,13 @@
         <v>0.57</v>
       </c>
       <c r="B59" t="n">
-        <v>465340</v>
+        <v>4692</v>
       </c>
       <c r="C59" t="n">
-        <v>6295</v>
+        <v>4954</v>
       </c>
       <c r="D59" t="n">
-        <v>0.006295</v>
+        <v>0.4954</v>
       </c>
       <c r="E59" t="inlineStr"/>
     </row>
@@ -1335,13 +1335,13 @@
         <v>0.58</v>
       </c>
       <c r="B60" t="n">
-        <v>451536</v>
+        <v>4583</v>
       </c>
       <c r="C60" t="n">
-        <v>10192</v>
+        <v>5039</v>
       </c>
       <c r="D60" t="n">
-        <v>0.010192</v>
+        <v>0.5039</v>
       </c>
       <c r="E60" t="inlineStr"/>
     </row>
@@ -1350,13 +1350,13 @@
         <v>0.59</v>
       </c>
       <c r="B61" t="n">
-        <v>438041</v>
+        <v>4495</v>
       </c>
       <c r="C61" t="n">
-        <v>44630</v>
+        <v>5139</v>
       </c>
       <c r="D61" t="n">
-        <v>0.04463</v>
+        <v>0.5139</v>
       </c>
       <c r="E61" t="inlineStr"/>
     </row>
@@ -1365,13 +1365,13 @@
         <v>0.6</v>
       </c>
       <c r="B62" t="n">
-        <v>425204</v>
+        <v>4410</v>
       </c>
       <c r="C62" t="n">
-        <v>104061</v>
+        <v>5233</v>
       </c>
       <c r="D62" t="n">
-        <v>0.104061</v>
+        <v>0.5233</v>
       </c>
       <c r="E62" t="inlineStr"/>
     </row>
@@ -1380,13 +1380,13 @@
         <v>0.61</v>
       </c>
       <c r="B63" t="n">
-        <v>412297</v>
+        <v>4310</v>
       </c>
       <c r="C63" t="n">
-        <v>440333</v>
+        <v>5322</v>
       </c>
       <c r="D63" t="n">
-        <v>0.440333</v>
+        <v>0.5322</v>
       </c>
       <c r="E63" t="inlineStr"/>
     </row>
@@ -1395,13 +1395,13 @@
         <v>0.62</v>
       </c>
       <c r="B64" t="n">
-        <v>399774</v>
+        <v>4205</v>
       </c>
       <c r="C64" t="n">
-        <v>517755</v>
+        <v>5412</v>
       </c>
       <c r="D64" t="n">
-        <v>0.517755</v>
+        <v>0.5412</v>
       </c>
       <c r="E64" t="inlineStr"/>
     </row>
@@ -1410,13 +1410,13 @@
         <v>0.63</v>
       </c>
       <c r="B65" t="n">
-        <v>387676</v>
+        <v>4085</v>
       </c>
       <c r="C65" t="n">
-        <v>554462</v>
+        <v>5515</v>
       </c>
       <c r="D65" t="n">
-        <v>0.554462</v>
+        <v>0.5515</v>
       </c>
       <c r="E65" t="inlineStr"/>
     </row>
@@ -1425,13 +1425,13 @@
         <v>0.64</v>
       </c>
       <c r="B66" t="n">
-        <v>375603</v>
+        <v>3985</v>
       </c>
       <c r="C66" t="n">
-        <v>578589</v>
+        <v>5626</v>
       </c>
       <c r="D66" t="n">
-        <v>0.578589</v>
+        <v>0.5626</v>
       </c>
       <c r="E66" t="inlineStr"/>
     </row>
@@ -1440,13 +1440,13 @@
         <v>0.65</v>
       </c>
       <c r="B67" t="n">
-        <v>363786</v>
+        <v>3888</v>
       </c>
       <c r="C67" t="n">
-        <v>599244</v>
+        <v>5717</v>
       </c>
       <c r="D67" t="n">
-        <v>0.599244</v>
+        <v>0.5717</v>
       </c>
       <c r="E67" t="inlineStr"/>
     </row>
@@ -1455,13 +1455,13 @@
         <v>0.66</v>
       </c>
       <c r="B68" t="n">
-        <v>352001</v>
+        <v>3764</v>
       </c>
       <c r="C68" t="n">
-        <v>618174</v>
+        <v>5838</v>
       </c>
       <c r="D68" t="n">
-        <v>0.618174</v>
+        <v>0.5838</v>
       </c>
       <c r="E68" t="inlineStr"/>
     </row>
@@ -1470,13 +1470,13 @@
         <v>0.67</v>
       </c>
       <c r="B69" t="n">
-        <v>340491</v>
+        <v>3662</v>
       </c>
       <c r="C69" t="n">
-        <v>634421</v>
+        <v>5963</v>
       </c>
       <c r="D69" t="n">
-        <v>0.634421</v>
+        <v>0.5963000000000001</v>
       </c>
       <c r="E69" t="inlineStr"/>
     </row>
@@ -1485,13 +1485,13 @@
         <v>0.68</v>
       </c>
       <c r="B70" t="n">
-        <v>329168</v>
+        <v>3582</v>
       </c>
       <c r="C70" t="n">
-        <v>648923</v>
+        <v>6048</v>
       </c>
       <c r="D70" t="n">
-        <v>0.648923</v>
+        <v>0.6048</v>
       </c>
       <c r="E70" t="inlineStr"/>
     </row>
@@ -1500,13 +1500,13 @@
         <v>0.6899999999999999</v>
       </c>
       <c r="B71" t="n">
-        <v>317985</v>
+        <v>3481</v>
       </c>
       <c r="C71" t="n">
-        <v>662946</v>
+        <v>6114</v>
       </c>
       <c r="D71" t="n">
-        <v>0.662946</v>
+        <v>0.6114000000000001</v>
       </c>
       <c r="E71" t="inlineStr"/>
     </row>
@@ -1515,13 +1515,13 @@
         <v>0.7</v>
       </c>
       <c r="B72" t="n">
-        <v>307015</v>
+        <v>3149</v>
       </c>
       <c r="C72" t="n">
-        <v>676293</v>
+        <v>6572</v>
       </c>
       <c r="D72" t="n">
-        <v>0.676293</v>
+        <v>0.6572</v>
       </c>
       <c r="E72" t="inlineStr"/>
     </row>
@@ -1530,13 +1530,13 @@
         <v>0.71</v>
       </c>
       <c r="B73" t="n">
-        <v>296017</v>
+        <v>3061</v>
       </c>
       <c r="C73" t="n">
-        <v>688700</v>
+        <v>6665</v>
       </c>
       <c r="D73" t="n">
-        <v>0.6887</v>
+        <v>0.6665</v>
       </c>
       <c r="E73" t="inlineStr"/>
     </row>
@@ -1545,13 +1545,13 @@
         <v>0.72</v>
       </c>
       <c r="B74" t="n">
-        <v>285096</v>
+        <v>2949</v>
       </c>
       <c r="C74" t="n">
-        <v>701000</v>
+        <v>6783</v>
       </c>
       <c r="D74" t="n">
-        <v>0.701</v>
+        <v>0.6783</v>
       </c>
       <c r="E74" t="inlineStr"/>
     </row>
@@ -1560,13 +1560,13 @@
         <v>0.73</v>
       </c>
       <c r="B75" t="n">
-        <v>274453</v>
+        <v>2838</v>
       </c>
       <c r="C75" t="n">
-        <v>712733</v>
+        <v>6908</v>
       </c>
       <c r="D75" t="n">
-        <v>0.7127329999999999</v>
+        <v>0.6908</v>
       </c>
       <c r="E75" t="inlineStr"/>
     </row>
@@ -1575,13 +1575,13 @@
         <v>0.74</v>
       </c>
       <c r="B76" t="n">
-        <v>263851</v>
+        <v>2721</v>
       </c>
       <c r="C76" t="n">
-        <v>723999</v>
+        <v>7022</v>
       </c>
       <c r="D76" t="n">
-        <v>0.7239989999999999</v>
+        <v>0.7022</v>
       </c>
       <c r="E76" t="inlineStr"/>
     </row>
@@ -1590,13 +1590,13 @@
         <v>0.75</v>
       </c>
       <c r="B77" t="n">
-        <v>253286</v>
+        <v>2616</v>
       </c>
       <c r="C77" t="n">
-        <v>735013</v>
+        <v>7138</v>
       </c>
       <c r="D77" t="n">
-        <v>0.735013</v>
+        <v>0.7138</v>
       </c>
       <c r="E77" t="inlineStr"/>
     </row>
@@ -1605,13 +1605,13 @@
         <v>0.76</v>
       </c>
       <c r="B78" t="n">
-        <v>242729</v>
+        <v>2499</v>
       </c>
       <c r="C78" t="n">
-        <v>745958</v>
+        <v>7263</v>
       </c>
       <c r="D78" t="n">
-        <v>0.745958</v>
+        <v>0.7262999999999999</v>
       </c>
       <c r="E78" t="inlineStr"/>
     </row>
@@ -1620,13 +1620,13 @@
         <v>0.77</v>
       </c>
       <c r="B79" t="n">
-        <v>232141</v>
+        <v>2401</v>
       </c>
       <c r="C79" t="n">
-        <v>756890</v>
+        <v>7376</v>
       </c>
       <c r="D79" t="n">
-        <v>0.75689</v>
+        <v>0.7376</v>
       </c>
       <c r="E79" t="inlineStr"/>
     </row>
@@ -1635,13 +1635,13 @@
         <v>0.78</v>
       </c>
       <c r="B80" t="n">
-        <v>221611</v>
+        <v>2290</v>
       </c>
       <c r="C80" t="n">
-        <v>767651</v>
+        <v>7472</v>
       </c>
       <c r="D80" t="n">
-        <v>0.767651</v>
+        <v>0.7472</v>
       </c>
       <c r="E80" t="inlineStr"/>
     </row>
@@ -1650,13 +1650,13 @@
         <v>0.79</v>
       </c>
       <c r="B81" t="n">
-        <v>211199</v>
+        <v>2195</v>
       </c>
       <c r="C81" t="n">
-        <v>778395</v>
+        <v>7577</v>
       </c>
       <c r="D81" t="n">
-        <v>0.7783949999999999</v>
+        <v>0.7577</v>
       </c>
       <c r="E81" t="inlineStr"/>
     </row>
@@ -1665,13 +1665,13 @@
         <v>0.8</v>
       </c>
       <c r="B82" t="n">
-        <v>200966</v>
+        <v>2090</v>
       </c>
       <c r="C82" t="n">
-        <v>788902</v>
+        <v>7676</v>
       </c>
       <c r="D82" t="n">
-        <v>0.788902</v>
+        <v>0.7675999999999999</v>
       </c>
       <c r="E82" t="inlineStr"/>
     </row>
@@ -1680,13 +1680,13 @@
         <v>0.8100000000000001</v>
       </c>
       <c r="B83" t="n">
-        <v>190645</v>
+        <v>1986</v>
       </c>
       <c r="C83" t="n">
-        <v>799252</v>
+        <v>7798</v>
       </c>
       <c r="D83" t="n">
-        <v>0.799252</v>
+        <v>0.7798</v>
       </c>
       <c r="E83" t="inlineStr"/>
     </row>
@@ -1695,13 +1695,13 @@
         <v>0.82</v>
       </c>
       <c r="B84" t="n">
-        <v>180463</v>
+        <v>1894</v>
       </c>
       <c r="C84" t="n">
-        <v>809623</v>
+        <v>7911</v>
       </c>
       <c r="D84" t="n">
-        <v>0.809623</v>
+        <v>0.7911</v>
       </c>
       <c r="E84" t="inlineStr"/>
     </row>
@@ -1710,13 +1710,13 @@
         <v>0.83</v>
       </c>
       <c r="B85" t="n">
-        <v>170337</v>
+        <v>1791</v>
       </c>
       <c r="C85" t="n">
-        <v>819899</v>
+        <v>7997</v>
       </c>
       <c r="D85" t="n">
-        <v>0.819899</v>
+        <v>0.7997</v>
       </c>
       <c r="E85" t="inlineStr"/>
     </row>
@@ -1725,13 +1725,13 @@
         <v>0.84</v>
       </c>
       <c r="B86" t="n">
-        <v>160331</v>
+        <v>1676</v>
       </c>
       <c r="C86" t="n">
-        <v>830036</v>
+        <v>8104</v>
       </c>
       <c r="D86" t="n">
-        <v>0.830036</v>
+        <v>0.8104</v>
       </c>
       <c r="E86" t="inlineStr"/>
     </row>
@@ -1740,13 +1740,13 @@
         <v>0.85</v>
       </c>
       <c r="B87" t="n">
-        <v>150331</v>
+        <v>1584</v>
       </c>
       <c r="C87" t="n">
-        <v>840067</v>
+        <v>8226</v>
       </c>
       <c r="D87" t="n">
-        <v>0.840067</v>
+        <v>0.8226</v>
       </c>
       <c r="E87" t="inlineStr"/>
     </row>
@@ -1755,13 +1755,13 @@
         <v>0.86</v>
       </c>
       <c r="B88" t="n">
-        <v>140403</v>
+        <v>1494</v>
       </c>
       <c r="C88" t="n">
-        <v>850091</v>
+        <v>8320</v>
       </c>
       <c r="D88" t="n">
-        <v>0.850091</v>
+        <v>0.832</v>
       </c>
       <c r="E88" t="inlineStr"/>
     </row>
@@ -1770,13 +1770,13 @@
         <v>0.87</v>
       </c>
       <c r="B89" t="n">
-        <v>130451</v>
+        <v>1380</v>
       </c>
       <c r="C89" t="n">
-        <v>860033</v>
+        <v>8421</v>
       </c>
       <c r="D89" t="n">
-        <v>0.860033</v>
+        <v>0.8421</v>
       </c>
       <c r="E89" t="inlineStr"/>
     </row>
@@ -1785,13 +1785,13 @@
         <v>0.88</v>
       </c>
       <c r="B90" t="n">
-        <v>120313</v>
+        <v>1261</v>
       </c>
       <c r="C90" t="n">
-        <v>869996</v>
+        <v>8541</v>
       </c>
       <c r="D90" t="n">
-        <v>0.869996</v>
+        <v>0.8541</v>
       </c>
       <c r="E90" t="inlineStr"/>
     </row>
@@ -1800,13 +1800,13 @@
         <v>0.89</v>
       </c>
       <c r="B91" t="n">
-        <v>110303</v>
+        <v>1168</v>
       </c>
       <c r="C91" t="n">
-        <v>880165</v>
+        <v>8686</v>
       </c>
       <c r="D91" t="n">
-        <v>0.880165</v>
+        <v>0.8686</v>
       </c>
       <c r="E91" t="inlineStr"/>
     </row>
@@ -1815,13 +1815,13 @@
         <v>0.9</v>
       </c>
       <c r="B92" t="n">
-        <v>100336</v>
+        <v>1080</v>
       </c>
       <c r="C92" t="n">
-        <v>890141</v>
+        <v>8772</v>
       </c>
       <c r="D92" t="n">
-        <v>0.890141</v>
+        <v>0.8772</v>
       </c>
       <c r="E92" t="inlineStr"/>
     </row>
@@ -1830,13 +1830,13 @@
         <v>0.91</v>
       </c>
       <c r="B93" t="n">
-        <v>90353</v>
+        <v>978</v>
       </c>
       <c r="C93" t="n">
-        <v>900142</v>
+        <v>8867</v>
       </c>
       <c r="D93" t="n">
-        <v>0.900142</v>
+        <v>0.8867</v>
       </c>
       <c r="E93" t="inlineStr"/>
     </row>
@@ -1845,13 +1845,13 @@
         <v>0.92</v>
       </c>
       <c r="B94" t="n">
-        <v>80289</v>
+        <v>871</v>
       </c>
       <c r="C94" t="n">
-        <v>910109</v>
+        <v>8984</v>
       </c>
       <c r="D94" t="n">
-        <v>0.9101089999999999</v>
+        <v>0.8984</v>
       </c>
       <c r="E94" t="inlineStr"/>
     </row>
@@ -1860,13 +1860,13 @@
         <v>0.93</v>
       </c>
       <c r="B95" t="n">
-        <v>70256</v>
+        <v>768</v>
       </c>
       <c r="C95" t="n">
-        <v>920150</v>
+        <v>9092</v>
       </c>
       <c r="D95" t="n">
-        <v>0.92015</v>
+        <v>0.9092</v>
       </c>
       <c r="E95" t="inlineStr"/>
     </row>
@@ -1875,13 +1875,13 @@
         <v>0.9399999999999999</v>
       </c>
       <c r="B96" t="n">
-        <v>60121</v>
+        <v>668</v>
       </c>
       <c r="C96" t="n">
-        <v>930219</v>
+        <v>9229</v>
       </c>
       <c r="D96" t="n">
-        <v>0.930219</v>
+        <v>0.9229000000000001</v>
       </c>
       <c r="E96" t="inlineStr"/>
     </row>
@@ -1890,13 +1890,13 @@
         <v>0.95</v>
       </c>
       <c r="B97" t="n">
-        <v>50193</v>
+        <v>535</v>
       </c>
       <c r="C97" t="n">
-        <v>940323</v>
+        <v>9326</v>
       </c>
       <c r="D97" t="n">
-        <v>0.940323</v>
+        <v>0.9326</v>
       </c>
       <c r="E97" t="inlineStr"/>
     </row>
@@ -1905,13 +1905,13 @@
         <v>0.96</v>
       </c>
       <c r="B98" t="n">
-        <v>40031</v>
+        <v>428</v>
       </c>
       <c r="C98" t="n">
-        <v>950291</v>
+        <v>9462</v>
       </c>
       <c r="D98" t="n">
-        <v>0.950291</v>
+        <v>0.9462</v>
       </c>
       <c r="E98" t="inlineStr"/>
     </row>
@@ -1920,13 +1920,13 @@
         <v>0.97</v>
       </c>
       <c r="B99" t="n">
-        <v>30029</v>
+        <v>324</v>
       </c>
       <c r="C99" t="n">
-        <v>960451</v>
+        <v>9563</v>
       </c>
       <c r="D99" t="n">
-        <v>0.9604510000000001</v>
+        <v>0.9563</v>
       </c>
       <c r="E99" t="inlineStr"/>
     </row>
@@ -1935,13 +1935,13 @@
         <v>0.98</v>
       </c>
       <c r="B100" t="n">
-        <v>19920</v>
+        <v>227</v>
       </c>
       <c r="C100" t="n">
-        <v>970443</v>
+        <v>9679</v>
       </c>
       <c r="D100" t="n">
-        <v>0.9704429999999999</v>
+        <v>0.9679</v>
       </c>
       <c r="E100" t="inlineStr"/>
     </row>
@@ -1950,13 +1950,13 @@
         <v>0.99</v>
       </c>
       <c r="B101" t="n">
-        <v>10104</v>
+        <v>114</v>
       </c>
       <c r="C101" t="n">
-        <v>980555</v>
+        <v>9786</v>
       </c>
       <c r="D101" t="n">
-        <v>0.980555</v>
+        <v>0.9786</v>
       </c>
       <c r="E101" t="inlineStr"/>
     </row>
@@ -1968,10 +1968,10 @@
         <v>1</v>
       </c>
       <c r="C102" t="n">
-        <v>990366</v>
+        <v>9904</v>
       </c>
       <c r="D102" t="n">
-        <v>0.990366</v>
+        <v>0.9903999999999999</v>
       </c>
       <c r="E102" t="inlineStr"/>
     </row>
@@ -1987,13 +1987,13 @@
         <v>0</v>
       </c>
       <c r="B104" t="n">
-        <v>1000000</v>
+        <v>10000</v>
       </c>
       <c r="C104" t="n">
         <v>1</v>
       </c>
       <c r="D104" t="n">
-        <v>1e-06</v>
+        <v>0.0001</v>
       </c>
       <c r="E104" t="inlineStr"/>
     </row>
@@ -2002,13 +2002,13 @@
         <v>0.01</v>
       </c>
       <c r="B105" t="n">
-        <v>999798</v>
+        <v>9989</v>
       </c>
       <c r="C105" t="n">
         <v>3</v>
       </c>
       <c r="D105" t="n">
-        <v>3e-06</v>
+        <v>0.0003</v>
       </c>
       <c r="E105" t="inlineStr"/>
     </row>
@@ -2017,13 +2017,13 @@
         <v>0.02</v>
       </c>
       <c r="B106" t="n">
-        <v>999160</v>
+        <v>9957</v>
       </c>
       <c r="C106" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D106" t="n">
-        <v>3e-06</v>
+        <v>0.0005</v>
       </c>
       <c r="E106" t="inlineStr"/>
     </row>
@@ -2032,13 +2032,13 @@
         <v>0.03</v>
       </c>
       <c r="B107" t="n">
-        <v>998147</v>
+        <v>9903</v>
       </c>
       <c r="C107" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D107" t="n">
-        <v>5e-06</v>
+        <v>0.0007</v>
       </c>
       <c r="E107" t="inlineStr"/>
     </row>
@@ -2047,13 +2047,13 @@
         <v>0.04</v>
       </c>
       <c r="B108" t="n">
-        <v>996763</v>
+        <v>9817</v>
       </c>
       <c r="C108" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D108" t="n">
-        <v>6e-06</v>
+        <v>0.0022</v>
       </c>
       <c r="E108" t="inlineStr"/>
     </row>
@@ -2062,13 +2062,13 @@
         <v>0.05</v>
       </c>
       <c r="B109" t="n">
-        <v>995005</v>
+        <v>9733</v>
       </c>
       <c r="C109" t="n">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D109" t="n">
-        <v>6e-06</v>
+        <v>0.0024</v>
       </c>
       <c r="E109" t="inlineStr"/>
     </row>
@@ -2077,13 +2077,13 @@
         <v>0.06</v>
       </c>
       <c r="B110" t="n">
-        <v>992737</v>
+        <v>9628</v>
       </c>
       <c r="C110" t="n">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="D110" t="n">
-        <v>6e-06</v>
+        <v>0.0031</v>
       </c>
       <c r="E110" t="inlineStr"/>
     </row>
@@ -2092,13 +2092,13 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="B111" t="n">
-        <v>990158</v>
+        <v>9532</v>
       </c>
       <c r="C111" t="n">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="D111" t="n">
-        <v>7e-06</v>
+        <v>0.0034</v>
       </c>
       <c r="E111" t="inlineStr"/>
     </row>
@@ -2107,13 +2107,13 @@
         <v>0.08</v>
       </c>
       <c r="B112" t="n">
-        <v>987162</v>
+        <v>9422</v>
       </c>
       <c r="C112" t="n">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="D112" t="n">
-        <v>8e-06</v>
+        <v>0.005</v>
       </c>
       <c r="E112" t="inlineStr"/>
     </row>
@@ -2122,13 +2122,13 @@
         <v>0.09</v>
       </c>
       <c r="B113" t="n">
-        <v>983804</v>
+        <v>9322</v>
       </c>
       <c r="C113" t="n">
-        <v>9</v>
+        <v>318</v>
       </c>
       <c r="D113" t="n">
-        <v>9e-06</v>
+        <v>0.0318</v>
       </c>
       <c r="E113" t="inlineStr"/>
     </row>
@@ -2137,13 +2137,13 @@
         <v>0.1</v>
       </c>
       <c r="B114" t="n">
-        <v>980153</v>
+        <v>9230</v>
       </c>
       <c r="C114" t="n">
-        <v>10</v>
+        <v>401</v>
       </c>
       <c r="D114" t="n">
-        <v>1e-05</v>
+        <v>0.0401</v>
       </c>
       <c r="E114" t="inlineStr"/>
     </row>
@@ -2152,13 +2152,13 @@
         <v>0.11</v>
       </c>
       <c r="B115" t="n">
-        <v>975884</v>
+        <v>9103</v>
       </c>
       <c r="C115" t="n">
-        <v>10</v>
+        <v>523</v>
       </c>
       <c r="D115" t="n">
-        <v>1e-05</v>
+        <v>0.0523</v>
       </c>
       <c r="E115" t="inlineStr"/>
     </row>
@@ -2167,13 +2167,13 @@
         <v>0.12</v>
       </c>
       <c r="B116" t="n">
-        <v>971285</v>
+        <v>9012</v>
       </c>
       <c r="C116" t="n">
-        <v>12</v>
+        <v>671</v>
       </c>
       <c r="D116" t="n">
-        <v>1.2e-05</v>
+        <v>0.06710000000000001</v>
       </c>
       <c r="E116" t="inlineStr"/>
     </row>
@@ -2182,13 +2182,13 @@
         <v>0.13</v>
       </c>
       <c r="B117" t="n">
-        <v>966426</v>
+        <v>8909</v>
       </c>
       <c r="C117" t="n">
-        <v>12</v>
+        <v>742</v>
       </c>
       <c r="D117" t="n">
-        <v>1.2e-05</v>
+        <v>0.0742</v>
       </c>
       <c r="E117" t="inlineStr"/>
     </row>
@@ -2197,13 +2197,13 @@
         <v>0.14</v>
       </c>
       <c r="B118" t="n">
-        <v>961053</v>
+        <v>8786</v>
       </c>
       <c r="C118" t="n">
-        <v>12</v>
+        <v>806</v>
       </c>
       <c r="D118" t="n">
-        <v>1.2e-05</v>
+        <v>0.0806</v>
       </c>
       <c r="E118" t="inlineStr"/>
     </row>
@@ -2212,13 +2212,13 @@
         <v>0.15</v>
       </c>
       <c r="B119" t="n">
-        <v>955424</v>
+        <v>8673</v>
       </c>
       <c r="C119" t="n">
-        <v>13</v>
+        <v>966</v>
       </c>
       <c r="D119" t="n">
-        <v>1.3e-05</v>
+        <v>0.09660000000000001</v>
       </c>
       <c r="E119" t="inlineStr"/>
     </row>
@@ -2227,13 +2227,13 @@
         <v>0.16</v>
       </c>
       <c r="B120" t="n">
-        <v>949542</v>
+        <v>8579</v>
       </c>
       <c r="C120" t="n">
-        <v>13</v>
+        <v>1083</v>
       </c>
       <c r="D120" t="n">
-        <v>1.3e-05</v>
+        <v>0.1083</v>
       </c>
       <c r="E120" t="inlineStr"/>
     </row>
@@ -2242,13 +2242,13 @@
         <v>0.17</v>
       </c>
       <c r="B121" t="n">
-        <v>943135</v>
+        <v>8487</v>
       </c>
       <c r="C121" t="n">
-        <v>14</v>
+        <v>1162</v>
       </c>
       <c r="D121" t="n">
-        <v>1.4e-05</v>
+        <v>0.1162</v>
       </c>
       <c r="E121" t="inlineStr"/>
     </row>
@@ -2257,13 +2257,13 @@
         <v>0.18</v>
       </c>
       <c r="B122" t="n">
-        <v>936495</v>
+        <v>8378</v>
       </c>
       <c r="C122" t="n">
-        <v>17</v>
+        <v>1289</v>
       </c>
       <c r="D122" t="n">
-        <v>1.7e-05</v>
+        <v>0.1289</v>
       </c>
       <c r="E122" t="inlineStr"/>
     </row>
@@ -2272,13 +2272,13 @@
         <v>0.19</v>
       </c>
       <c r="B123" t="n">
-        <v>929311</v>
+        <v>8278</v>
       </c>
       <c r="C123" t="n">
-        <v>23</v>
+        <v>1391</v>
       </c>
       <c r="D123" t="n">
-        <v>2.3e-05</v>
+        <v>0.1391</v>
       </c>
       <c r="E123" t="inlineStr"/>
     </row>
@@ -2287,13 +2287,13 @@
         <v>0.2</v>
       </c>
       <c r="B124" t="n">
-        <v>922029</v>
+        <v>8175</v>
       </c>
       <c r="C124" t="n">
-        <v>24</v>
+        <v>1485</v>
       </c>
       <c r="D124" t="n">
-        <v>2.4e-05</v>
+        <v>0.1485</v>
       </c>
       <c r="E124" t="inlineStr"/>
     </row>
@@ -2302,13 +2302,13 @@
         <v>0.21</v>
       </c>
       <c r="B125" t="n">
-        <v>914340</v>
+        <v>8063</v>
       </c>
       <c r="C125" t="n">
-        <v>27</v>
+        <v>1581</v>
       </c>
       <c r="D125" t="n">
-        <v>2.7e-05</v>
+        <v>0.1581</v>
       </c>
       <c r="E125" t="inlineStr"/>
     </row>
@@ -2317,13 +2317,13 @@
         <v>0.22</v>
       </c>
       <c r="B126" t="n">
-        <v>906288</v>
+        <v>7958</v>
       </c>
       <c r="C126" t="n">
-        <v>27</v>
+        <v>1687</v>
       </c>
       <c r="D126" t="n">
-        <v>2.7e-05</v>
+        <v>0.1687</v>
       </c>
       <c r="E126" t="inlineStr"/>
     </row>
@@ -2332,13 +2332,13 @@
         <v>0.23</v>
       </c>
       <c r="B127" t="n">
-        <v>897784</v>
+        <v>7845</v>
       </c>
       <c r="C127" t="n">
-        <v>27</v>
+        <v>1800</v>
       </c>
       <c r="D127" t="n">
-        <v>2.7e-05</v>
+        <v>0.18</v>
       </c>
       <c r="E127" t="inlineStr"/>
     </row>
@@ -2347,13 +2347,13 @@
         <v>0.24</v>
       </c>
       <c r="B128" t="n">
-        <v>889218</v>
+        <v>7732</v>
       </c>
       <c r="C128" t="n">
-        <v>28</v>
+        <v>1874</v>
       </c>
       <c r="D128" t="n">
-        <v>2.8e-05</v>
+        <v>0.1874</v>
       </c>
       <c r="E128" t="inlineStr"/>
     </row>
@@ -2362,13 +2362,13 @@
         <v>0.25</v>
       </c>
       <c r="B129" t="n">
-        <v>879855</v>
+        <v>7631</v>
       </c>
       <c r="C129" t="n">
-        <v>28</v>
+        <v>2028</v>
       </c>
       <c r="D129" t="n">
-        <v>2.8e-05</v>
+        <v>0.2028</v>
       </c>
       <c r="E129" t="inlineStr"/>
     </row>
@@ -2377,13 +2377,13 @@
         <v>0.26</v>
       </c>
       <c r="B130" t="n">
-        <v>870461</v>
+        <v>7528</v>
       </c>
       <c r="C130" t="n">
-        <v>29</v>
+        <v>2123</v>
       </c>
       <c r="D130" t="n">
-        <v>2.9e-05</v>
+        <v>0.2123</v>
       </c>
       <c r="E130" t="inlineStr"/>
     </row>
@@ -2392,13 +2392,13 @@
         <v>0.27</v>
       </c>
       <c r="B131" t="n">
-        <v>860673</v>
+        <v>7408</v>
       </c>
       <c r="C131" t="n">
-        <v>32</v>
+        <v>2247</v>
       </c>
       <c r="D131" t="n">
-        <v>3.2e-05</v>
+        <v>0.2247</v>
       </c>
       <c r="E131" t="inlineStr"/>
     </row>
@@ -2407,13 +2407,13 @@
         <v>0.28</v>
       </c>
       <c r="B132" t="n">
-        <v>850577</v>
+        <v>7319</v>
       </c>
       <c r="C132" t="n">
-        <v>36</v>
+        <v>2333</v>
       </c>
       <c r="D132" t="n">
-        <v>3.6e-05</v>
+        <v>0.2333</v>
       </c>
       <c r="E132" t="inlineStr"/>
     </row>
@@ -2422,13 +2422,13 @@
         <v>0.29</v>
       </c>
       <c r="B133" t="n">
-        <v>840266</v>
+        <v>7209</v>
       </c>
       <c r="C133" t="n">
-        <v>39</v>
+        <v>2436</v>
       </c>
       <c r="D133" t="n">
-        <v>3.9e-05</v>
+        <v>0.2436</v>
       </c>
       <c r="E133" t="inlineStr"/>
     </row>
@@ -2437,13 +2437,13 @@
         <v>0.3</v>
       </c>
       <c r="B134" t="n">
-        <v>829721</v>
+        <v>7111</v>
       </c>
       <c r="C134" t="n">
-        <v>44</v>
+        <v>2533</v>
       </c>
       <c r="D134" t="n">
-        <v>4.4e-05</v>
+        <v>0.2533</v>
       </c>
       <c r="E134" t="inlineStr"/>
     </row>
@@ -2452,13 +2452,13 @@
         <v>0.31</v>
       </c>
       <c r="B135" t="n">
-        <v>818738</v>
+        <v>7004</v>
       </c>
       <c r="C135" t="n">
-        <v>50</v>
+        <v>2622</v>
       </c>
       <c r="D135" t="n">
-        <v>5e-05</v>
+        <v>0.2622</v>
       </c>
       <c r="E135" t="inlineStr"/>
     </row>
@@ -2467,13 +2467,13 @@
         <v>0.32</v>
       </c>
       <c r="B136" t="n">
-        <v>807229</v>
+        <v>6908</v>
       </c>
       <c r="C136" t="n">
-        <v>50</v>
+        <v>2739</v>
       </c>
       <c r="D136" t="n">
-        <v>5e-05</v>
+        <v>0.2739</v>
       </c>
       <c r="E136" t="inlineStr"/>
     </row>
@@ -2482,13 +2482,13 @@
         <v>0.33</v>
       </c>
       <c r="B137" t="n">
-        <v>795951</v>
+        <v>6817</v>
       </c>
       <c r="C137" t="n">
-        <v>50</v>
+        <v>2815</v>
       </c>
       <c r="D137" t="n">
-        <v>5e-05</v>
+        <v>0.2815</v>
       </c>
       <c r="E137" t="inlineStr"/>
     </row>
@@ -2497,13 +2497,13 @@
         <v>0.34</v>
       </c>
       <c r="B138" t="n">
-        <v>784043</v>
+        <v>6723</v>
       </c>
       <c r="C138" t="n">
-        <v>59</v>
+        <v>2954</v>
       </c>
       <c r="D138" t="n">
-        <v>5.9e-05</v>
+        <v>0.2954</v>
       </c>
       <c r="E138" t="inlineStr"/>
     </row>
@@ -2512,13 +2512,13 @@
         <v>0.35</v>
       </c>
       <c r="B139" t="n">
-        <v>771796</v>
+        <v>6623</v>
       </c>
       <c r="C139" t="n">
-        <v>62</v>
+        <v>3066</v>
       </c>
       <c r="D139" t="n">
-        <v>6.2e-05</v>
+        <v>0.3066</v>
       </c>
       <c r="E139" t="inlineStr"/>
     </row>
@@ -2527,13 +2527,13 @@
         <v>0.36</v>
       </c>
       <c r="B140" t="n">
-        <v>759522</v>
+        <v>6516</v>
       </c>
       <c r="C140" t="n">
-        <v>69</v>
+        <v>3185</v>
       </c>
       <c r="D140" t="n">
-        <v>6.9e-05</v>
+        <v>0.3185</v>
       </c>
       <c r="E140" t="inlineStr"/>
     </row>
@@ -2542,13 +2542,13 @@
         <v>0.37</v>
       </c>
       <c r="B141" t="n">
-        <v>746932</v>
+        <v>6407</v>
       </c>
       <c r="C141" t="n">
-        <v>83</v>
+        <v>3289</v>
       </c>
       <c r="D141" t="n">
-        <v>8.3e-05</v>
+        <v>0.3289</v>
       </c>
       <c r="E141" t="inlineStr"/>
     </row>
@@ -2557,13 +2557,13 @@
         <v>0.38</v>
       </c>
       <c r="B142" t="n">
-        <v>734067</v>
+        <v>6318</v>
       </c>
       <c r="C142" t="n">
-        <v>90</v>
+        <v>3390</v>
       </c>
       <c r="D142" t="n">
-        <v>9.000000000000001e-05</v>
+        <v>0.339</v>
       </c>
       <c r="E142" t="inlineStr"/>
     </row>
@@ -2572,13 +2572,13 @@
         <v>0.39</v>
       </c>
       <c r="B143" t="n">
-        <v>721175</v>
+        <v>6217</v>
       </c>
       <c r="C143" t="n">
-        <v>90</v>
+        <v>3498</v>
       </c>
       <c r="D143" t="n">
-        <v>9.000000000000001e-05</v>
+        <v>0.3498</v>
       </c>
       <c r="E143" t="inlineStr"/>
     </row>
@@ -2587,13 +2587,13 @@
         <v>0.4</v>
       </c>
       <c r="B144" t="n">
-        <v>708086</v>
+        <v>6135</v>
       </c>
       <c r="C144" t="n">
-        <v>107</v>
+        <v>3582</v>
       </c>
       <c r="D144" t="n">
-        <v>0.000107</v>
+        <v>0.3582</v>
       </c>
       <c r="E144" t="inlineStr"/>
     </row>
@@ -2602,13 +2602,13 @@
         <v>0.41</v>
       </c>
       <c r="B145" t="n">
-        <v>694671</v>
+        <v>6042</v>
       </c>
       <c r="C145" t="n">
-        <v>156</v>
+        <v>3655</v>
       </c>
       <c r="D145" t="n">
-        <v>0.000156</v>
+        <v>0.3655</v>
       </c>
       <c r="E145" t="inlineStr"/>
     </row>
@@ -2617,13 +2617,13 @@
         <v>0.42</v>
       </c>
       <c r="B146" t="n">
-        <v>680958</v>
+        <v>5936</v>
       </c>
       <c r="C146" t="n">
-        <v>159</v>
+        <v>3767</v>
       </c>
       <c r="D146" t="n">
-        <v>0.000159</v>
+        <v>0.3767</v>
       </c>
       <c r="E146" t="inlineStr"/>
     </row>
@@ -2632,13 +2632,13 @@
         <v>0.43</v>
       </c>
       <c r="B147" t="n">
-        <v>667431</v>
+        <v>5856</v>
       </c>
       <c r="C147" t="n">
-        <v>168</v>
+        <v>3842</v>
       </c>
       <c r="D147" t="n">
-        <v>0.000168</v>
+        <v>0.3842</v>
       </c>
       <c r="E147" t="inlineStr"/>
     </row>
@@ -2647,13 +2647,13 @@
         <v>0.44</v>
       </c>
       <c r="B148" t="n">
-        <v>653460</v>
+        <v>5741</v>
       </c>
       <c r="C148" t="n">
-        <v>171</v>
+        <v>3944</v>
       </c>
       <c r="D148" t="n">
-        <v>0.000171</v>
+        <v>0.3944</v>
       </c>
       <c r="E148" t="inlineStr"/>
     </row>
@@ -2662,13 +2662,13 @@
         <v>0.45</v>
       </c>
       <c r="B149" t="n">
-        <v>639518</v>
+        <v>5650</v>
       </c>
       <c r="C149" t="n">
-        <v>189</v>
+        <v>4052</v>
       </c>
       <c r="D149" t="n">
-        <v>0.000189</v>
+        <v>0.4052</v>
       </c>
       <c r="E149" t="inlineStr"/>
     </row>
@@ -2677,13 +2677,13 @@
         <v>0.46</v>
       </c>
       <c r="B150" t="n">
-        <v>625240</v>
+        <v>5544</v>
       </c>
       <c r="C150" t="n">
-        <v>233</v>
+        <v>4169</v>
       </c>
       <c r="D150" t="n">
-        <v>0.000233</v>
+        <v>0.4169</v>
       </c>
       <c r="E150" t="inlineStr"/>
     </row>
@@ -2692,13 +2692,13 @@
         <v>0.47</v>
       </c>
       <c r="B151" t="n">
-        <v>611064</v>
+        <v>5435</v>
       </c>
       <c r="C151" t="n">
-        <v>297</v>
+        <v>4274</v>
       </c>
       <c r="D151" t="n">
-        <v>0.000297</v>
+        <v>0.4274</v>
       </c>
       <c r="E151" t="inlineStr"/>
     </row>
@@ -2707,13 +2707,13 @@
         <v>0.48</v>
       </c>
       <c r="B152" t="n">
-        <v>596770</v>
+        <v>5338</v>
       </c>
       <c r="C152" t="n">
-        <v>334</v>
+        <v>4390</v>
       </c>
       <c r="D152" t="n">
-        <v>0.000334</v>
+        <v>0.439</v>
       </c>
       <c r="E152" t="inlineStr"/>
     </row>
@@ -2722,13 +2722,13 @@
         <v>0.49</v>
       </c>
       <c r="B153" t="n">
-        <v>582408</v>
+        <v>5247</v>
       </c>
       <c r="C153" t="n">
-        <v>409</v>
+        <v>4471</v>
       </c>
       <c r="D153" t="n">
-        <v>0.000409</v>
+        <v>0.4471</v>
       </c>
       <c r="E153" t="inlineStr"/>
     </row>
@@ -2737,13 +2737,13 @@
         <v>0.5</v>
       </c>
       <c r="B154" t="n">
-        <v>567993</v>
+        <v>5131</v>
       </c>
       <c r="C154" t="n">
-        <v>488</v>
+        <v>4587</v>
       </c>
       <c r="D154" t="n">
-        <v>0.000488</v>
+        <v>0.4587</v>
       </c>
       <c r="E154" t="inlineStr"/>
     </row>
@@ -2752,13 +2752,13 @@
         <v>0.51</v>
       </c>
       <c r="B155" t="n">
-        <v>553455</v>
+        <v>5041</v>
       </c>
       <c r="C155" t="n">
-        <v>501</v>
+        <v>4673</v>
       </c>
       <c r="D155" t="n">
-        <v>0.000501</v>
+        <v>0.4673</v>
       </c>
       <c r="E155" t="inlineStr"/>
     </row>
@@ -2767,13 +2767,13 @@
         <v>0.52</v>
       </c>
       <c r="B156" t="n">
-        <v>538948</v>
+        <v>4912</v>
       </c>
       <c r="C156" t="n">
-        <v>729</v>
+        <v>4798</v>
       </c>
       <c r="D156" t="n">
-        <v>0.000729</v>
+        <v>0.4798</v>
       </c>
       <c r="E156" t="inlineStr"/>
     </row>
@@ -2782,13 +2782,13 @@
         <v>0.53</v>
       </c>
       <c r="B157" t="n">
-        <v>524637</v>
+        <v>4817</v>
       </c>
       <c r="C157" t="n">
-        <v>905</v>
+        <v>4919</v>
       </c>
       <c r="D157" t="n">
-        <v>0.000905</v>
+        <v>0.4919</v>
       </c>
       <c r="E157" t="inlineStr"/>
     </row>
@@ -2797,13 +2797,13 @@
         <v>0.54</v>
       </c>
       <c r="B158" t="n">
-        <v>510548</v>
+        <v>4722</v>
       </c>
       <c r="C158" t="n">
-        <v>1111</v>
+        <v>5011</v>
       </c>
       <c r="D158" t="n">
-        <v>0.001111</v>
+        <v>0.5011</v>
       </c>
       <c r="E158" t="inlineStr"/>
     </row>
@@ -2812,13 +2812,13 @@
         <v>0.55</v>
       </c>
       <c r="B159" t="n">
-        <v>496072</v>
+        <v>4616</v>
       </c>
       <c r="C159" t="n">
-        <v>1562</v>
+        <v>5106</v>
       </c>
       <c r="D159" t="n">
-        <v>0.001562</v>
+        <v>0.5106000000000001</v>
       </c>
       <c r="E159" t="inlineStr"/>
     </row>
@@ -2827,13 +2827,13 @@
         <v>0.5600000000000001</v>
       </c>
       <c r="B160" t="n">
-        <v>481766</v>
+        <v>4525</v>
       </c>
       <c r="C160" t="n">
-        <v>3046</v>
+        <v>5219</v>
       </c>
       <c r="D160" t="n">
-        <v>0.003046</v>
+        <v>0.5219</v>
       </c>
       <c r="E160" t="inlineStr"/>
     </row>
@@ -2842,13 +2842,13 @@
         <v>0.57</v>
       </c>
       <c r="B161" t="n">
-        <v>467878</v>
+        <v>4412</v>
       </c>
       <c r="C161" t="n">
-        <v>7992</v>
+        <v>5330</v>
       </c>
       <c r="D161" t="n">
-        <v>0.007992000000000001</v>
+        <v>0.533</v>
       </c>
       <c r="E161" t="inlineStr"/>
     </row>
@@ -2857,13 +2857,13 @@
         <v>0.58</v>
       </c>
       <c r="B162" t="n">
-        <v>454106</v>
+        <v>4330</v>
       </c>
       <c r="C162" t="n">
-        <v>20649</v>
+        <v>5425</v>
       </c>
       <c r="D162" t="n">
-        <v>0.020649</v>
+        <v>0.5425</v>
       </c>
       <c r="E162" t="inlineStr"/>
     </row>
@@ -2872,13 +2872,13 @@
         <v>0.59</v>
       </c>
       <c r="B163" t="n">
-        <v>440516</v>
+        <v>4235</v>
       </c>
       <c r="C163" t="n">
-        <v>41645</v>
+        <v>5519</v>
       </c>
       <c r="D163" t="n">
-        <v>0.041645</v>
+        <v>0.5518999999999999</v>
       </c>
       <c r="E163" t="inlineStr"/>
     </row>
@@ -2887,13 +2887,13 @@
         <v>0.6</v>
       </c>
       <c r="B164" t="n">
-        <v>427116</v>
+        <v>4124</v>
       </c>
       <c r="C164" t="n">
-        <v>354810</v>
+        <v>5611</v>
       </c>
       <c r="D164" t="n">
-        <v>0.35481</v>
+        <v>0.5611</v>
       </c>
       <c r="E164" t="inlineStr"/>
     </row>
@@ -2902,13 +2902,13 @@
         <v>0.61</v>
       </c>
       <c r="B165" t="n">
-        <v>414400</v>
+        <v>4014</v>
       </c>
       <c r="C165" t="n">
-        <v>464595</v>
+        <v>5724</v>
       </c>
       <c r="D165" t="n">
-        <v>0.464595</v>
+        <v>0.5724</v>
       </c>
       <c r="E165" t="inlineStr"/>
     </row>
@@ -2917,13 +2917,13 @@
         <v>0.62</v>
       </c>
       <c r="B166" t="n">
-        <v>401716</v>
+        <v>3919</v>
       </c>
       <c r="C166" t="n">
-        <v>523292</v>
+        <v>5824</v>
       </c>
       <c r="D166" t="n">
-        <v>0.523292</v>
+        <v>0.5824</v>
       </c>
       <c r="E166" t="inlineStr"/>
     </row>
@@ -2932,13 +2932,13 @@
         <v>0.63</v>
       </c>
       <c r="B167" t="n">
-        <v>389404</v>
+        <v>3816</v>
       </c>
       <c r="C167" t="n">
-        <v>556701</v>
+        <v>5921</v>
       </c>
       <c r="D167" t="n">
-        <v>0.556701</v>
+        <v>0.5921</v>
       </c>
       <c r="E167" t="inlineStr"/>
     </row>
@@ -2947,13 +2947,13 @@
         <v>0.64</v>
       </c>
       <c r="B168" t="n">
-        <v>377268</v>
+        <v>3698</v>
       </c>
       <c r="C168" t="n">
-        <v>582896</v>
+        <v>6044</v>
       </c>
       <c r="D168" t="n">
-        <v>0.582896</v>
+        <v>0.6044</v>
       </c>
       <c r="E168" t="inlineStr"/>
     </row>
@@ -2962,13 +2962,13 @@
         <v>0.65</v>
       </c>
       <c r="B169" t="n">
-        <v>365526</v>
+        <v>3608</v>
       </c>
       <c r="C169" t="n">
-        <v>604467</v>
+        <v>6151</v>
       </c>
       <c r="D169" t="n">
-        <v>0.604467</v>
+        <v>0.6151</v>
       </c>
       <c r="E169" t="inlineStr"/>
     </row>
@@ -2977,13 +2977,13 @@
         <v>0.66</v>
       </c>
       <c r="B170" t="n">
-        <v>353717</v>
+        <v>3517</v>
       </c>
       <c r="C170" t="n">
-        <v>622867</v>
+        <v>6241</v>
       </c>
       <c r="D170" t="n">
-        <v>0.6228669999999999</v>
+        <v>0.6241</v>
       </c>
       <c r="E170" t="inlineStr"/>
     </row>
@@ -2992,13 +2992,13 @@
         <v>0.67</v>
       </c>
       <c r="B171" t="n">
-        <v>342193</v>
+        <v>3417</v>
       </c>
       <c r="C171" t="n">
-        <v>639640</v>
+        <v>6343</v>
       </c>
       <c r="D171" t="n">
-        <v>0.63964</v>
+        <v>0.6343</v>
       </c>
       <c r="E171" t="inlineStr"/>
     </row>
@@ -3007,13 +3007,13 @@
         <v>0.68</v>
       </c>
       <c r="B172" t="n">
-        <v>330564</v>
+        <v>3343</v>
       </c>
       <c r="C172" t="n">
-        <v>654303</v>
+        <v>6439</v>
       </c>
       <c r="D172" t="n">
-        <v>0.654303</v>
+        <v>0.6439</v>
       </c>
       <c r="E172" t="inlineStr"/>
     </row>
@@ -3022,13 +3022,13 @@
         <v>0.6899999999999999</v>
       </c>
       <c r="B173" t="n">
-        <v>319088</v>
+        <v>3247</v>
       </c>
       <c r="C173" t="n">
-        <v>668014</v>
+        <v>6552</v>
       </c>
       <c r="D173" t="n">
-        <v>0.668014</v>
+        <v>0.6552</v>
       </c>
       <c r="E173" t="inlineStr"/>
     </row>
@@ -3037,13 +3037,13 @@
         <v>0.7</v>
       </c>
       <c r="B174" t="n">
-        <v>308009</v>
+        <v>3141</v>
       </c>
       <c r="C174" t="n">
-        <v>681048</v>
+        <v>6656</v>
       </c>
       <c r="D174" t="n">
-        <v>0.681048</v>
+        <v>0.6656</v>
       </c>
       <c r="E174" t="inlineStr"/>
     </row>
@@ -3052,13 +3052,13 @@
         <v>0.71</v>
       </c>
       <c r="B175" t="n">
-        <v>296961</v>
+        <v>3024</v>
       </c>
       <c r="C175" t="n">
-        <v>693425</v>
+        <v>6769</v>
       </c>
       <c r="D175" t="n">
-        <v>0.693425</v>
+        <v>0.6768999999999999</v>
       </c>
       <c r="E175" t="inlineStr"/>
     </row>
@@ -3067,13 +3067,13 @@
         <v>0.72</v>
       </c>
       <c r="B176" t="n">
-        <v>286025</v>
+        <v>2926</v>
       </c>
       <c r="C176" t="n">
-        <v>705535</v>
+        <v>6913</v>
       </c>
       <c r="D176" t="n">
-        <v>0.705535</v>
+        <v>0.6913</v>
       </c>
       <c r="E176" t="inlineStr"/>
     </row>
@@ -3082,13 +3082,13 @@
         <v>0.73</v>
       </c>
       <c r="B177" t="n">
-        <v>275048</v>
+        <v>2830</v>
       </c>
       <c r="C177" t="n">
-        <v>717417</v>
+        <v>7006</v>
       </c>
       <c r="D177" t="n">
-        <v>0.717417</v>
+        <v>0.7006</v>
       </c>
       <c r="E177" t="inlineStr"/>
     </row>
@@ -3097,13 +3097,13 @@
         <v>0.74</v>
       </c>
       <c r="B178" t="n">
-        <v>264210</v>
+        <v>2729</v>
       </c>
       <c r="C178" t="n">
-        <v>728925</v>
+        <v>7112</v>
       </c>
       <c r="D178" t="n">
-        <v>0.728925</v>
+        <v>0.7112000000000001</v>
       </c>
       <c r="E178" t="inlineStr"/>
     </row>
@@ -3112,13 +3112,13 @@
         <v>0.75</v>
       </c>
       <c r="B179" t="n">
-        <v>253663</v>
+        <v>2619</v>
       </c>
       <c r="C179" t="n">
-        <v>740057</v>
+        <v>7221</v>
       </c>
       <c r="D179" t="n">
-        <v>0.740057</v>
+        <v>0.7221</v>
       </c>
       <c r="E179" t="inlineStr"/>
     </row>
@@ -3127,13 +3127,13 @@
         <v>0.76</v>
       </c>
       <c r="B180" t="n">
-        <v>243064</v>
+        <v>2518</v>
       </c>
       <c r="C180" t="n">
-        <v>751035</v>
+        <v>7328</v>
       </c>
       <c r="D180" t="n">
-        <v>0.751035</v>
+        <v>0.7328</v>
       </c>
       <c r="E180" t="inlineStr"/>
     </row>
@@ -3142,13 +3142,13 @@
         <v>0.77</v>
       </c>
       <c r="B181" t="n">
-        <v>232630</v>
+        <v>2425</v>
       </c>
       <c r="C181" t="n">
-        <v>761837</v>
+        <v>7439</v>
       </c>
       <c r="D181" t="n">
-        <v>0.761837</v>
+        <v>0.7439</v>
       </c>
       <c r="E181" t="inlineStr"/>
     </row>
@@ -3157,13 +3157,13 @@
         <v>0.78</v>
       </c>
       <c r="B182" t="n">
-        <v>222031</v>
+        <v>2325</v>
       </c>
       <c r="C182" t="n">
-        <v>772565</v>
+        <v>7536</v>
       </c>
       <c r="D182" t="n">
-        <v>0.7725649999999999</v>
+        <v>0.7536</v>
       </c>
       <c r="E182" t="inlineStr"/>
     </row>
@@ -3172,13 +3172,13 @@
         <v>0.79</v>
       </c>
       <c r="B183" t="n">
-        <v>211497</v>
+        <v>2210</v>
       </c>
       <c r="C183" t="n">
-        <v>783386</v>
+        <v>7664</v>
       </c>
       <c r="D183" t="n">
-        <v>0.783386</v>
+        <v>0.7664</v>
       </c>
       <c r="E183" t="inlineStr"/>
     </row>
@@ -3187,13 +3187,13 @@
         <v>0.8</v>
       </c>
       <c r="B184" t="n">
-        <v>201245</v>
+        <v>2093</v>
       </c>
       <c r="C184" t="n">
-        <v>793805</v>
+        <v>7800</v>
       </c>
       <c r="D184" t="n">
-        <v>0.793805</v>
+        <v>0.78</v>
       </c>
       <c r="E184" t="inlineStr"/>
     </row>
@@ -3202,13 +3202,13 @@
         <v>0.8100000000000001</v>
       </c>
       <c r="B185" t="n">
-        <v>190961</v>
+        <v>1993</v>
       </c>
       <c r="C185" t="n">
-        <v>804116</v>
+        <v>7902</v>
       </c>
       <c r="D185" t="n">
-        <v>0.8041160000000001</v>
+        <v>0.7902</v>
       </c>
       <c r="E185" t="inlineStr"/>
     </row>
@@ -3217,13 +3217,13 @@
         <v>0.82</v>
       </c>
       <c r="B186" t="n">
-        <v>180698</v>
+        <v>1883</v>
       </c>
       <c r="C186" t="n">
-        <v>814593</v>
+        <v>8009</v>
       </c>
       <c r="D186" t="n">
-        <v>0.814593</v>
+        <v>0.8008999999999999</v>
       </c>
       <c r="E186" t="inlineStr"/>
     </row>
@@ -3232,13 +3232,13 @@
         <v>0.83</v>
       </c>
       <c r="B187" t="n">
-        <v>170453</v>
+        <v>1781</v>
       </c>
       <c r="C187" t="n">
-        <v>824907</v>
+        <v>8115</v>
       </c>
       <c r="D187" t="n">
-        <v>0.8249069999999999</v>
+        <v>0.8115</v>
       </c>
       <c r="E187" t="inlineStr"/>
     </row>
@@ -3247,13 +3247,13 @@
         <v>0.84</v>
       </c>
       <c r="B188" t="n">
-        <v>160393</v>
+        <v>1691</v>
       </c>
       <c r="C188" t="n">
-        <v>835050</v>
+        <v>8228</v>
       </c>
       <c r="D188" t="n">
-        <v>0.83505</v>
+        <v>0.8228</v>
       </c>
       <c r="E188" t="inlineStr"/>
     </row>
@@ -3262,13 +3262,13 @@
         <v>0.85</v>
       </c>
       <c r="B189" t="n">
-        <v>150333</v>
+        <v>1580</v>
       </c>
       <c r="C189" t="n">
-        <v>845048</v>
+        <v>8338</v>
       </c>
       <c r="D189" t="n">
-        <v>0.845048</v>
+        <v>0.8338</v>
       </c>
       <c r="E189" t="inlineStr"/>
     </row>
@@ -3277,13 +3277,13 @@
         <v>0.86</v>
       </c>
       <c r="B190" t="n">
-        <v>140112</v>
+        <v>1484</v>
       </c>
       <c r="C190" t="n">
-        <v>855241</v>
+        <v>8446</v>
       </c>
       <c r="D190" t="n">
-        <v>0.855241</v>
+        <v>0.8446</v>
       </c>
       <c r="E190" t="inlineStr"/>
     </row>
@@ -3292,13 +3292,13 @@
         <v>0.87</v>
       </c>
       <c r="B191" t="n">
-        <v>129933</v>
+        <v>1376</v>
       </c>
       <c r="C191" t="n">
-        <v>865429</v>
+        <v>8557</v>
       </c>
       <c r="D191" t="n">
-        <v>0.865429</v>
+        <v>0.8557</v>
       </c>
       <c r="E191" t="inlineStr"/>
     </row>
@@ -3307,13 +3307,13 @@
         <v>0.88</v>
       </c>
       <c r="B192" t="n">
-        <v>119890</v>
+        <v>1272</v>
       </c>
       <c r="C192" t="n">
-        <v>875486</v>
+        <v>8668</v>
       </c>
       <c r="D192" t="n">
-        <v>0.875486</v>
+        <v>0.8668</v>
       </c>
       <c r="E192" t="inlineStr"/>
     </row>
@@ -3322,13 +3322,13 @@
         <v>0.89</v>
       </c>
       <c r="B193" t="n">
-        <v>109612</v>
+        <v>1146</v>
       </c>
       <c r="C193" t="n">
-        <v>885726</v>
+        <v>8795</v>
       </c>
       <c r="D193" t="n">
-        <v>0.885726</v>
+        <v>0.8794999999999999</v>
       </c>
       <c r="E193" t="inlineStr"/>
     </row>
@@ -3337,13 +3337,13 @@
         <v>0.9</v>
       </c>
       <c r="B194" t="n">
-        <v>99693</v>
+        <v>1041</v>
       </c>
       <c r="C194" t="n">
-        <v>895857</v>
+        <v>8898</v>
       </c>
       <c r="D194" t="n">
-        <v>0.895857</v>
+        <v>0.8898</v>
       </c>
       <c r="E194" t="inlineStr"/>
     </row>
@@ -3352,13 +3352,13 @@
         <v>0.91</v>
       </c>
       <c r="B195" t="n">
-        <v>89730</v>
+        <v>940</v>
       </c>
       <c r="C195" t="n">
-        <v>905784</v>
+        <v>9006</v>
       </c>
       <c r="D195" t="n">
-        <v>0.905784</v>
+        <v>0.9006</v>
       </c>
       <c r="E195" t="inlineStr"/>
     </row>
@@ -3367,13 +3367,13 @@
         <v>0.92</v>
       </c>
       <c r="B196" t="n">
-        <v>79673</v>
+        <v>839</v>
       </c>
       <c r="C196" t="n">
-        <v>915879</v>
+        <v>9105</v>
       </c>
       <c r="D196" t="n">
-        <v>0.915879</v>
+        <v>0.9105</v>
       </c>
       <c r="E196" t="inlineStr"/>
     </row>
@@ -3382,13 +3382,13 @@
         <v>0.93</v>
       </c>
       <c r="B197" t="n">
-        <v>69736</v>
+        <v>714</v>
       </c>
       <c r="C197" t="n">
-        <v>925838</v>
+        <v>9233</v>
       </c>
       <c r="D197" t="n">
-        <v>0.925838</v>
+        <v>0.9233</v>
       </c>
       <c r="E197" t="inlineStr"/>
     </row>
@@ -3397,13 +3397,13 @@
         <v>0.9399999999999999</v>
       </c>
       <c r="B198" t="n">
-        <v>59763</v>
+        <v>611</v>
       </c>
       <c r="C198" t="n">
-        <v>935826</v>
+        <v>9338</v>
       </c>
       <c r="D198" t="n">
-        <v>0.935826</v>
+        <v>0.9338</v>
       </c>
       <c r="E198" t="inlineStr"/>
     </row>
@@ -3412,13 +3412,13 @@
         <v>0.95</v>
       </c>
       <c r="B199" t="n">
-        <v>49814</v>
+        <v>524</v>
       </c>
       <c r="C199" t="n">
-        <v>945751</v>
+        <v>9449</v>
       </c>
       <c r="D199" t="n">
-        <v>0.945751</v>
+        <v>0.9449</v>
       </c>
       <c r="E199" t="inlineStr"/>
     </row>
@@ -3427,13 +3427,13 @@
         <v>0.96</v>
       </c>
       <c r="B200" t="n">
-        <v>39997</v>
+        <v>436</v>
       </c>
       <c r="C200" t="n">
-        <v>955685</v>
+        <v>9531</v>
       </c>
       <c r="D200" t="n">
-        <v>0.955685</v>
+        <v>0.9530999999999999</v>
       </c>
       <c r="E200" t="inlineStr"/>
     </row>
@@ -3442,13 +3442,13 @@
         <v>0.97</v>
       </c>
       <c r="B201" t="n">
-        <v>30080</v>
+        <v>297</v>
       </c>
       <c r="C201" t="n">
-        <v>965482</v>
+        <v>9678</v>
       </c>
       <c r="D201" t="n">
-        <v>0.965482</v>
+        <v>0.9678</v>
       </c>
       <c r="E201" t="inlineStr"/>
     </row>
@@ -3457,13 +3457,13 @@
         <v>0.98</v>
       </c>
       <c r="B202" t="n">
-        <v>20048</v>
+        <v>209</v>
       </c>
       <c r="C202" t="n">
-        <v>975517</v>
+        <v>9775</v>
       </c>
       <c r="D202" t="n">
-        <v>0.975517</v>
+        <v>0.9775</v>
       </c>
       <c r="E202" t="inlineStr"/>
     </row>
@@ -3472,13 +3472,13 @@
         <v>0.99</v>
       </c>
       <c r="B203" t="n">
-        <v>10051</v>
+        <v>103</v>
       </c>
       <c r="C203" t="n">
-        <v>985388</v>
+        <v>9874</v>
       </c>
       <c r="D203" t="n">
-        <v>0.985388</v>
+        <v>0.9874000000000001</v>
       </c>
       <c r="E203" t="inlineStr"/>
     </row>
@@ -3490,10 +3490,10 @@
         <v>1</v>
       </c>
       <c r="C204" t="n">
-        <v>995456</v>
+        <v>9993</v>
       </c>
       <c r="D204" t="n">
-        <v>0.995456</v>
+        <v>0.9993</v>
       </c>
       <c r="E204" t="inlineStr"/>
     </row>
@@ -3503,7 +3503,7 @@
       <c r="C205" t="inlineStr"/>
       <c r="D205" t="inlineStr"/>
       <c r="E205" t="n">
-        <v>0.6</v>
+        <v>0.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>